<commit_message>
Update SPR example, restore old examples
</commit_message>
<xml_diff>
--- a/examples/spr-submission-invalid-highlighted.xlsx
+++ b/examples/spr-submission-invalid-highlighted.xlsx
@@ -421,77 +421,77 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>- Antibody label: TODO</t>
+          <t>- Antibody label: the COVIC label for the antibody (e.g. COVIC 1)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>- Tested antigen: TODO</t>
+          <t>- Tested antigen: the name of the tested antigen (e.g. Spike protein 1)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>- n: TODO</t>
+          <t>- n: the number of runs for the assay (e.g. 6)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>- on rate; Ka in M^-1s^-1: TODO</t>
+          <t>- on rate; Ka in M^-1s^-1: an SPR assay measuring on rate [Ka] in M^-1s^-1 (e.g. 491000)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>- Standard deviation in M^-1s^-1: TODO</t>
+          <t>- Standard deviation in M^-1s^-1: The standard deviation of the value in 'Standard deviation in M^-1s^-1'</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>- off rate; Kd in 1/s: TODO</t>
+          <t>- off rate; Kd in 1/s: an SPR assay measuring off rate [Kd] in 1/s (e.g. 126)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>- Standard deviation in 1/s: TODO</t>
+          <t>- Standard deviation in 1/s: The standard deviation of the value in 'Standard deviation in 1/s'</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>- dissociation constant; KD in nM: TODO</t>
+          <t>- dissociation constant; KD in nM: an SPR assay measuring dissociation constant [KD] in nM (e.g. &lt;.1)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>- Standard deviation in nM: TODO</t>
+          <t>- Standard deviation in nM: The standard deviation of the value in 'Standard deviation in nM'</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>- Qualitiative measure: TODO</t>
+          <t>- Qualitiative measure: the qualitative measure of the assay (e.g. positive)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>- Comment: TODO</t>
+          <t>- Comment: general comments about the assay (e.g. did not bind positive control)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve ab_* validation for assays
</commit_message>
<xml_diff>
--- a/examples/spr-submission-invalid-highlighted.xlsx
+++ b/examples/spr-submission-invalid-highlighted.xlsx
@@ -75,6 +75,11 @@
     <author>Validation service</author>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A2" shapeId="0">
+      <text>
+        <t>'COVIC 1' is not a valid COVIC antibody label in column 'Antibody label'</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="C2" shapeId="0">
       <text>
         <t>'X' is not of type 'integer' in column 'n'</t>
@@ -587,7 +592,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>COVIC 1</t>
         </is>

</xml_diff>